<commit_message>
Updated: some roms visualization codes
</commit_message>
<xml_diff>
--- a/my_scripts/transect.xlsx
+++ b/my_scripts/transect.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bolinao_hypoxia\CCMS_data\animation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EE0D05-9703-4363-89FD-D9C50EEA7C2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB3BF02-2490-4C2D-9479-1E94B5F9498F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16470" windowHeight="9330" xr2:uid="{68DBF74F-1B36-4EFF-8658-3C9C1DBE3C27}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>transect1</t>
     <phoneticPr fontId="1"/>
@@ -46,23 +46,33 @@
     <t>transect3</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>transect4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>transect5</t>
+  </si>
+  <si>
+    <t>transect6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -408,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DBB84A2-4B23-417B-8F55-173E4F56F21E}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:E50"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +436,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -446,8 +465,26 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>43</v>
       </c>
@@ -466,8 +503,26 @@
       <c r="F3">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>108</v>
+      </c>
+      <c r="I3">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>137</v>
+      </c>
+      <c r="K3">
+        <v>82</v>
+      </c>
+      <c r="L3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>44</v>
       </c>
@@ -486,8 +541,26 @@
       <c r="F4">
         <v>135</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4">
+        <v>61</v>
+      </c>
+      <c r="H4">
+        <v>108</v>
+      </c>
+      <c r="I4">
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <v>137</v>
+      </c>
+      <c r="K4">
+        <v>82</v>
+      </c>
+      <c r="L4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>45</v>
       </c>
@@ -506,8 +579,26 @@
       <c r="F5">
         <v>135</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5">
+        <v>61</v>
+      </c>
+      <c r="H5">
+        <v>109</v>
+      </c>
+      <c r="I5">
+        <v>36</v>
+      </c>
+      <c r="J5">
+        <v>136</v>
+      </c>
+      <c r="K5">
+        <v>83</v>
+      </c>
+      <c r="L5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>45</v>
       </c>
@@ -526,8 +617,26 @@
       <c r="F6">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G6">
+        <v>62</v>
+      </c>
+      <c r="H6">
+        <v>109</v>
+      </c>
+      <c r="I6">
+        <v>36</v>
+      </c>
+      <c r="J6">
+        <v>135</v>
+      </c>
+      <c r="K6">
+        <v>83</v>
+      </c>
+      <c r="L6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>46</v>
       </c>
@@ -546,8 +655,26 @@
       <c r="F7">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G7">
+        <v>62</v>
+      </c>
+      <c r="H7">
+        <v>110</v>
+      </c>
+      <c r="I7">
+        <v>36</v>
+      </c>
+      <c r="J7">
+        <v>134</v>
+      </c>
+      <c r="K7">
+        <v>84</v>
+      </c>
+      <c r="L7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>46</v>
       </c>
@@ -566,8 +693,26 @@
       <c r="F8">
         <v>133</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <v>63</v>
+      </c>
+      <c r="H8">
+        <v>110</v>
+      </c>
+      <c r="I8">
+        <v>36</v>
+      </c>
+      <c r="J8">
+        <v>133</v>
+      </c>
+      <c r="K8">
+        <v>84</v>
+      </c>
+      <c r="L8">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>47</v>
       </c>
@@ -586,8 +731,26 @@
       <c r="F9">
         <v>133</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G9">
+        <v>63</v>
+      </c>
+      <c r="H9">
+        <v>111</v>
+      </c>
+      <c r="I9">
+        <v>36</v>
+      </c>
+      <c r="J9">
+        <v>132</v>
+      </c>
+      <c r="K9">
+        <v>85</v>
+      </c>
+      <c r="L9">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>47</v>
       </c>
@@ -606,8 +769,26 @@
       <c r="F10">
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G10">
+        <v>64</v>
+      </c>
+      <c r="H10">
+        <v>111</v>
+      </c>
+      <c r="I10">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <v>132</v>
+      </c>
+      <c r="K10">
+        <v>85</v>
+      </c>
+      <c r="L10">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>47</v>
       </c>
@@ -626,8 +807,26 @@
       <c r="F11">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G11">
+        <v>64</v>
+      </c>
+      <c r="H11">
+        <v>112</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+      <c r="J11">
+        <v>132</v>
+      </c>
+      <c r="K11">
+        <v>86</v>
+      </c>
+      <c r="L11">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>47</v>
       </c>
@@ -646,8 +845,26 @@
       <c r="F12">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G12">
+        <v>65</v>
+      </c>
+      <c r="H12">
+        <v>112</v>
+      </c>
+      <c r="I12">
+        <v>39</v>
+      </c>
+      <c r="J12">
+        <v>132</v>
+      </c>
+      <c r="K12">
+        <v>86</v>
+      </c>
+      <c r="L12">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>47</v>
       </c>
@@ -666,8 +883,26 @@
       <c r="F13">
         <v>129</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G13">
+        <v>65</v>
+      </c>
+      <c r="H13">
+        <v>113</v>
+      </c>
+      <c r="I13">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>132</v>
+      </c>
+      <c r="K13">
+        <v>87</v>
+      </c>
+      <c r="L13">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>47</v>
       </c>
@@ -686,8 +921,26 @@
       <c r="F14">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G14">
+        <v>66</v>
+      </c>
+      <c r="H14">
+        <v>113</v>
+      </c>
+      <c r="I14">
+        <v>40</v>
+      </c>
+      <c r="J14">
+        <v>133</v>
+      </c>
+      <c r="K14">
+        <v>87</v>
+      </c>
+      <c r="L14">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>47</v>
       </c>
@@ -706,8 +959,26 @@
       <c r="F15">
         <v>127</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G15">
+        <v>66</v>
+      </c>
+      <c r="H15">
+        <v>114</v>
+      </c>
+      <c r="I15">
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <v>134</v>
+      </c>
+      <c r="K15">
+        <v>88</v>
+      </c>
+      <c r="L15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>47</v>
       </c>
@@ -726,8 +997,26 @@
       <c r="F16">
         <v>126</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G16">
+        <v>67</v>
+      </c>
+      <c r="H16">
+        <v>114</v>
+      </c>
+      <c r="I16">
+        <v>41</v>
+      </c>
+      <c r="J16">
+        <v>134</v>
+      </c>
+      <c r="K16">
+        <v>88</v>
+      </c>
+      <c r="L16">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>48</v>
       </c>
@@ -746,8 +1035,26 @@
       <c r="F17">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G17">
+        <v>67</v>
+      </c>
+      <c r="H17">
+        <v>115</v>
+      </c>
+      <c r="I17">
+        <v>41</v>
+      </c>
+      <c r="J17">
+        <v>135</v>
+      </c>
+      <c r="K17">
+        <v>89</v>
+      </c>
+      <c r="L17">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>49</v>
       </c>
@@ -766,8 +1073,26 @@
       <c r="F18">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G18">
+        <v>68</v>
+      </c>
+      <c r="H18">
+        <v>115</v>
+      </c>
+      <c r="I18">
+        <v>42</v>
+      </c>
+      <c r="J18">
+        <v>135</v>
+      </c>
+      <c r="K18">
+        <v>89</v>
+      </c>
+      <c r="L18">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>49</v>
       </c>
@@ -786,8 +1111,26 @@
       <c r="F19">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G19">
+        <v>68</v>
+      </c>
+      <c r="H19">
+        <v>116</v>
+      </c>
+      <c r="I19">
+        <v>43</v>
+      </c>
+      <c r="J19">
+        <v>135</v>
+      </c>
+      <c r="K19">
+        <v>90</v>
+      </c>
+      <c r="L19">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>50</v>
       </c>
@@ -806,8 +1149,26 @@
       <c r="F20">
         <v>125</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G20">
+        <v>69</v>
+      </c>
+      <c r="H20">
+        <v>116</v>
+      </c>
+      <c r="I20">
+        <v>44</v>
+      </c>
+      <c r="J20">
+        <v>135</v>
+      </c>
+      <c r="K20">
+        <v>90</v>
+      </c>
+      <c r="L20">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>50</v>
       </c>
@@ -826,8 +1187,26 @@
       <c r="F21">
         <v>124</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G21">
+        <v>69</v>
+      </c>
+      <c r="H21">
+        <v>117</v>
+      </c>
+      <c r="I21">
+        <v>45</v>
+      </c>
+      <c r="J21">
+        <v>135</v>
+      </c>
+      <c r="K21">
+        <v>91</v>
+      </c>
+      <c r="L21">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>51</v>
       </c>
@@ -846,8 +1225,26 @@
       <c r="F22">
         <v>124</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G22">
+        <v>70</v>
+      </c>
+      <c r="H22">
+        <v>117</v>
+      </c>
+      <c r="I22">
+        <v>45</v>
+      </c>
+      <c r="J22">
+        <v>134</v>
+      </c>
+      <c r="K22">
+        <v>91</v>
+      </c>
+      <c r="L22">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>51</v>
       </c>
@@ -866,8 +1263,26 @@
       <c r="F23">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G23">
+        <v>70</v>
+      </c>
+      <c r="H23">
+        <v>118</v>
+      </c>
+      <c r="I23">
+        <v>46</v>
+      </c>
+      <c r="J23">
+        <v>134</v>
+      </c>
+      <c r="K23">
+        <v>92</v>
+      </c>
+      <c r="L23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>52</v>
       </c>
@@ -886,8 +1301,26 @@
       <c r="F24">
         <v>123</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G24">
+        <v>71</v>
+      </c>
+      <c r="H24">
+        <v>118</v>
+      </c>
+      <c r="I24">
+        <v>46</v>
+      </c>
+      <c r="J24">
+        <v>133</v>
+      </c>
+      <c r="K24">
+        <v>92</v>
+      </c>
+      <c r="L24">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>52</v>
       </c>
@@ -906,8 +1339,26 @@
       <c r="F25">
         <v>122</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G25">
+        <v>71</v>
+      </c>
+      <c r="H25">
+        <v>119</v>
+      </c>
+      <c r="I25">
+        <v>47</v>
+      </c>
+      <c r="J25">
+        <v>133</v>
+      </c>
+      <c r="K25">
+        <v>93</v>
+      </c>
+      <c r="L25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>52</v>
       </c>
@@ -926,8 +1377,26 @@
       <c r="F26">
         <v>121</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G26">
+        <v>72</v>
+      </c>
+      <c r="H26">
+        <v>119</v>
+      </c>
+      <c r="I26">
+        <v>47</v>
+      </c>
+      <c r="J26">
+        <v>132</v>
+      </c>
+      <c r="K26">
+        <v>93</v>
+      </c>
+      <c r="L26">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>53</v>
       </c>
@@ -946,8 +1415,26 @@
       <c r="F27">
         <v>121</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G27">
+        <v>72</v>
+      </c>
+      <c r="H27">
+        <v>120</v>
+      </c>
+      <c r="I27">
+        <v>47</v>
+      </c>
+      <c r="J27">
+        <v>131</v>
+      </c>
+      <c r="K27">
+        <v>94</v>
+      </c>
+      <c r="L27">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>53</v>
       </c>
@@ -966,8 +1453,26 @@
       <c r="F28">
         <v>120</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G28">
+        <v>73</v>
+      </c>
+      <c r="H28">
+        <v>120</v>
+      </c>
+      <c r="I28">
+        <v>47</v>
+      </c>
+      <c r="J28">
+        <v>130</v>
+      </c>
+      <c r="K28">
+        <v>94</v>
+      </c>
+      <c r="L28">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>54</v>
       </c>
@@ -986,8 +1491,26 @@
       <c r="F29">
         <v>119</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G29">
+        <v>73</v>
+      </c>
+      <c r="H29">
+        <v>121</v>
+      </c>
+      <c r="I29">
+        <v>47</v>
+      </c>
+      <c r="J29">
+        <v>129</v>
+      </c>
+      <c r="K29">
+        <v>95</v>
+      </c>
+      <c r="L29">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>54</v>
       </c>
@@ -1006,8 +1529,26 @@
       <c r="F30">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G30">
+        <v>74</v>
+      </c>
+      <c r="H30">
+        <v>121</v>
+      </c>
+      <c r="I30">
+        <v>47</v>
+      </c>
+      <c r="J30">
+        <v>128</v>
+      </c>
+      <c r="K30">
+        <v>95</v>
+      </c>
+      <c r="L30">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>55</v>
       </c>
@@ -1026,8 +1567,26 @@
       <c r="F31">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G31">
+        <v>74</v>
+      </c>
+      <c r="H31">
+        <v>122</v>
+      </c>
+      <c r="I31">
+        <v>47</v>
+      </c>
+      <c r="J31">
+        <v>127</v>
+      </c>
+      <c r="K31">
+        <v>96</v>
+      </c>
+      <c r="L31">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>55</v>
       </c>
@@ -1046,8 +1605,26 @@
       <c r="F32">
         <v>116</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G32">
+        <v>75</v>
+      </c>
+      <c r="H32">
+        <v>122</v>
+      </c>
+      <c r="I32">
+        <v>47</v>
+      </c>
+      <c r="J32">
+        <v>126</v>
+      </c>
+      <c r="K32">
+        <v>96</v>
+      </c>
+      <c r="L32">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>56</v>
       </c>
@@ -1066,8 +1643,26 @@
       <c r="F33">
         <v>115</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G33">
+        <v>75</v>
+      </c>
+      <c r="H33">
+        <v>123</v>
+      </c>
+      <c r="I33">
+        <v>48</v>
+      </c>
+      <c r="J33">
+        <v>126</v>
+      </c>
+      <c r="K33">
+        <v>97</v>
+      </c>
+      <c r="L33">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>56</v>
       </c>
@@ -1086,8 +1681,26 @@
       <c r="F34">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G34">
+        <v>76</v>
+      </c>
+      <c r="H34">
+        <v>123</v>
+      </c>
+      <c r="I34">
+        <v>49</v>
+      </c>
+      <c r="J34">
+        <v>126</v>
+      </c>
+      <c r="K34">
+        <v>97</v>
+      </c>
+      <c r="L34">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="C35">
         <v>54</v>
       </c>
@@ -1100,8 +1713,26 @@
       <c r="F35">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G35">
+        <v>76</v>
+      </c>
+      <c r="H35">
+        <v>124</v>
+      </c>
+      <c r="I35">
+        <v>49</v>
+      </c>
+      <c r="J35">
+        <v>125</v>
+      </c>
+      <c r="K35">
+        <v>98</v>
+      </c>
+      <c r="L35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="C36">
         <v>54</v>
       </c>
@@ -1114,8 +1745,26 @@
       <c r="F36">
         <v>112</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G36">
+        <v>77</v>
+      </c>
+      <c r="H36">
+        <v>124</v>
+      </c>
+      <c r="I36">
+        <v>50</v>
+      </c>
+      <c r="J36">
+        <v>125</v>
+      </c>
+      <c r="K36">
+        <v>98</v>
+      </c>
+      <c r="L36">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="C37">
         <v>54</v>
       </c>
@@ -1128,8 +1777,26 @@
       <c r="F37">
         <v>111</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G37">
+        <v>77</v>
+      </c>
+      <c r="H37">
+        <v>125</v>
+      </c>
+      <c r="I37">
+        <v>50</v>
+      </c>
+      <c r="J37">
+        <v>124</v>
+      </c>
+      <c r="K37">
+        <v>99</v>
+      </c>
+      <c r="L37">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="C38">
         <v>54</v>
       </c>
@@ -1142,8 +1809,26 @@
       <c r="F38">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G38">
+        <v>78</v>
+      </c>
+      <c r="H38">
+        <v>125</v>
+      </c>
+      <c r="I38">
+        <v>51</v>
+      </c>
+      <c r="J38">
+        <v>124</v>
+      </c>
+      <c r="K38">
+        <v>99</v>
+      </c>
+      <c r="L38">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="C39">
         <v>54</v>
       </c>
@@ -1156,8 +1841,26 @@
       <c r="F39">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G39">
+        <v>78</v>
+      </c>
+      <c r="H39">
+        <v>126</v>
+      </c>
+      <c r="I39">
+        <v>51</v>
+      </c>
+      <c r="J39">
+        <v>123</v>
+      </c>
+      <c r="K39">
+        <v>100</v>
+      </c>
+      <c r="L39">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="C40">
         <v>54</v>
       </c>
@@ -1170,8 +1873,26 @@
       <c r="F40">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G40">
+        <v>78</v>
+      </c>
+      <c r="H40">
+        <v>127</v>
+      </c>
+      <c r="I40">
+        <v>52</v>
+      </c>
+      <c r="J40">
+        <v>123</v>
+      </c>
+      <c r="K40">
+        <v>100</v>
+      </c>
+      <c r="L40">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="C41">
         <v>54</v>
       </c>
@@ -1184,8 +1905,26 @@
       <c r="F41">
         <v>107</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G41">
+        <v>79</v>
+      </c>
+      <c r="H41">
+        <v>127</v>
+      </c>
+      <c r="I41">
+        <v>52</v>
+      </c>
+      <c r="J41">
+        <v>122</v>
+      </c>
+      <c r="K41">
+        <v>101</v>
+      </c>
+      <c r="L41">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="C42">
         <v>55</v>
       </c>
@@ -1198,8 +1937,26 @@
       <c r="F42">
         <v>106</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G42">
+        <v>79</v>
+      </c>
+      <c r="H42">
+        <v>128</v>
+      </c>
+      <c r="I42">
+        <v>52</v>
+      </c>
+      <c r="J42">
+        <v>121</v>
+      </c>
+      <c r="K42">
+        <v>101</v>
+      </c>
+      <c r="L42">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="C43">
         <v>55</v>
       </c>
@@ -1212,8 +1969,26 @@
       <c r="F43">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G43">
+        <v>80</v>
+      </c>
+      <c r="H43">
+        <v>128</v>
+      </c>
+      <c r="I43">
+        <v>53</v>
+      </c>
+      <c r="J43">
+        <v>121</v>
+      </c>
+      <c r="K43">
+        <v>102</v>
+      </c>
+      <c r="L43">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="C44">
         <v>55</v>
       </c>
@@ -1226,8 +2001,26 @@
       <c r="F44">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G44">
+        <v>80</v>
+      </c>
+      <c r="H44">
+        <v>129</v>
+      </c>
+      <c r="I44">
+        <v>53</v>
+      </c>
+      <c r="J44">
+        <v>120</v>
+      </c>
+      <c r="K44">
+        <v>102</v>
+      </c>
+      <c r="L44">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="C45">
         <v>56</v>
       </c>
@@ -1240,8 +2033,26 @@
       <c r="F45">
         <v>103</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G45">
+        <v>81</v>
+      </c>
+      <c r="H45">
+        <v>129</v>
+      </c>
+      <c r="I45">
+        <v>54</v>
+      </c>
+      <c r="J45">
+        <v>120</v>
+      </c>
+      <c r="K45">
+        <v>103</v>
+      </c>
+      <c r="L45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="C46">
         <v>56</v>
       </c>
@@ -1254,8 +2065,26 @@
       <c r="F46">
         <v>102</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G46">
+        <v>81</v>
+      </c>
+      <c r="H46">
+        <v>130</v>
+      </c>
+      <c r="I46">
+        <v>54</v>
+      </c>
+      <c r="J46">
+        <v>119</v>
+      </c>
+      <c r="K46">
+        <v>103</v>
+      </c>
+      <c r="L46">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="C47">
         <v>56</v>
       </c>
@@ -1268,8 +2097,26 @@
       <c r="F47">
         <v>101</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G47">
+        <v>82</v>
+      </c>
+      <c r="H47">
+        <v>130</v>
+      </c>
+      <c r="I47">
+        <v>55</v>
+      </c>
+      <c r="J47">
+        <v>119</v>
+      </c>
+      <c r="K47">
+        <v>104</v>
+      </c>
+      <c r="L47">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="C48">
         <v>56</v>
       </c>
@@ -1282,8 +2129,26 @@
       <c r="F48">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="G48">
+        <v>82</v>
+      </c>
+      <c r="H48">
+        <v>131</v>
+      </c>
+      <c r="I48">
+        <v>55</v>
+      </c>
+      <c r="J48">
+        <v>118</v>
+      </c>
+      <c r="K48">
+        <v>104</v>
+      </c>
+      <c r="L48">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12">
       <c r="C49">
         <v>56</v>
       </c>
@@ -1296,13 +2161,65 @@
       <c r="F49">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.4">
+      <c r="G49">
+        <v>83</v>
+      </c>
+      <c r="H49">
+        <v>131</v>
+      </c>
+      <c r="I49">
+        <v>56</v>
+      </c>
+      <c r="J49">
+        <v>118</v>
+      </c>
+      <c r="K49">
+        <v>105</v>
+      </c>
+      <c r="L49">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12">
       <c r="E50">
         <v>53</v>
       </c>
       <c r="F50">
         <v>98</v>
+      </c>
+      <c r="G50">
+        <v>83</v>
+      </c>
+      <c r="H50">
+        <v>132</v>
+      </c>
+      <c r="I50">
+        <v>56</v>
+      </c>
+      <c r="J50">
+        <v>117</v>
+      </c>
+      <c r="K50">
+        <v>105</v>
+      </c>
+      <c r="L50">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12">
+      <c r="G51">
+        <v>84</v>
+      </c>
+      <c r="H51">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12">
+      <c r="G52">
+        <v>84</v>
+      </c>
+      <c r="H52">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>